<commit_message>
excel hz sprint 1 update
</commit_message>
<xml_diff>
--- a/TeamXXReport.xlsx
+++ b/TeamXXReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zildj\Documents\!School\6th Semester\Agile Methods\SSW555_Spring19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5033E60-59EB-43B5-B039-528AC7707261}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ADCDB70-0F93-4CB6-B618-5E535A8E2EB3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12040" yWindow="5300" windowWidth="24000" windowHeight="12760" tabRatio="500" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="5565" windowWidth="38700" windowHeight="15435" tabRatio="500" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="221">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -699,6 +699,42 @@
   </si>
   <si>
     <t>https://github.com/jjjpanda/SSW555_Spring19</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>hzSprint1.py</t>
+  </si>
+  <si>
+    <t>divorceBeforeDeath</t>
+  </si>
+  <si>
+    <t>test_US06.py</t>
+  </si>
+  <si>
+    <t>39-49</t>
+  </si>
+  <si>
+    <t>marriageAfterAge</t>
+  </si>
+  <si>
+    <t>5-12</t>
+  </si>
+  <si>
+    <t>15-27</t>
+  </si>
+  <si>
+    <t>test_US10.py</t>
+  </si>
+  <si>
+    <t>51-61</t>
+  </si>
+  <si>
+    <t>Object-Oriented design</t>
+  </si>
+  <si>
+    <t>Messy github directory</t>
   </si>
 </sst>
 </file>
@@ -867,7 +903,7 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -902,6 +938,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="65"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="67"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="66"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="68">
     <cellStyle name="Bad" xfId="67" builtinId="27"/>
@@ -2065,15 +2111,15 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.84375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.4609375" customWidth="1"/>
-    <col min="3" max="3" width="8.4609375" customWidth="1"/>
-    <col min="4" max="5" width="20.4609375" customWidth="1"/>
+    <col min="1" max="1" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5" customWidth="1"/>
+    <col min="3" max="3" width="8.5" customWidth="1"/>
+    <col min="4" max="5" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2090,7 +2136,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
         <v>182</v>
       </c>
@@ -2107,7 +2153,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>183</v>
       </c>
@@ -2124,7 +2170,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
         <v>184</v>
       </c>
@@ -2141,7 +2187,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
         <v>185</v>
       </c>
@@ -2158,10 +2204,10 @@
         <v>201</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E8" s="16"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D9" s="4" t="s">
         <v>34</v>
       </c>
@@ -2194,16 +2240,16 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.61328125" customWidth="1"/>
-    <col min="2" max="2" width="7.61328125" customWidth="1"/>
-    <col min="3" max="3" width="25.921875" customWidth="1"/>
-    <col min="4" max="4" width="6.921875" customWidth="1"/>
-    <col min="5" max="5" width="7.61328125" customWidth="1"/>
+    <col min="1" max="1" width="5.625" customWidth="1"/>
+    <col min="2" max="2" width="7.625" customWidth="1"/>
+    <col min="3" max="3" width="25.875" customWidth="1"/>
+    <col min="4" max="4" width="6.875" customWidth="1"/>
+    <col min="5" max="5" width="7.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>29</v>
       </c>
@@ -2220,7 +2266,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2237,7 +2283,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2254,7 +2300,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2271,7 +2317,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2288,7 +2334,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2305,7 +2351,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2322,7 +2368,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2339,7 +2385,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2356,7 +2402,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>119</v>
       </c>
@@ -2364,7 +2410,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>120</v>
       </c>
@@ -2372,7 +2418,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>122</v>
       </c>
@@ -2380,7 +2426,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>123</v>
       </c>
@@ -2388,7 +2434,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>125</v>
       </c>
@@ -2396,7 +2442,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>126</v>
       </c>
@@ -2404,7 +2450,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>129</v>
       </c>
@@ -2412,7 +2458,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>132</v>
       </c>
@@ -2420,7 +2466,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>133</v>
       </c>
@@ -2428,7 +2474,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>137</v>
       </c>
@@ -2436,7 +2482,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>138</v>
       </c>
@@ -2444,7 +2490,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>139</v>
       </c>
@@ -2452,7 +2498,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>140</v>
       </c>
@@ -2460,7 +2506,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>141</v>
       </c>
@@ -2468,7 +2514,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>142</v>
       </c>
@@ -2476,7 +2522,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>143</v>
       </c>
@@ -2484,7 +2530,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>144</v>
       </c>
@@ -2492,7 +2538,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>145</v>
       </c>
@@ -2500,7 +2546,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>146</v>
       </c>
@@ -2508,7 +2554,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>147</v>
       </c>
@@ -2516,7 +2562,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>148</v>
       </c>
@@ -2524,7 +2570,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>149</v>
       </c>
@@ -2532,7 +2578,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>150</v>
       </c>
@@ -2540,7 +2586,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>153</v>
       </c>
@@ -2566,47 +2612,47 @@
       <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.84375" style="2"/>
-    <col min="2" max="2" width="9.4609375" customWidth="1"/>
-    <col min="3" max="3" width="15.84375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.3828125" customWidth="1"/>
-    <col min="5" max="5" width="6.84375" customWidth="1"/>
-    <col min="6" max="6" width="12.4609375" style="7" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="2"/>
+    <col min="2" max="2" width="9.5" customWidth="1"/>
+    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.375" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>159</v>
       </c>
@@ -2629,7 +2675,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>160</v>
       </c>
@@ -2645,7 +2691,7 @@
       <c r="F15" s="12"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>161</v>
       </c>
@@ -2670,7 +2716,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>162</v>
       </c>
@@ -2695,7 +2741,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>163</v>
       </c>
@@ -2720,7 +2766,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>164</v>
       </c>
@@ -2760,17 +2806,17 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.84375" style="2"/>
-    <col min="2" max="2" width="16.61328125" customWidth="1"/>
-    <col min="3" max="3" width="12.4609375" customWidth="1"/>
-    <col min="4" max="4" width="7.15234375" customWidth="1"/>
-    <col min="5" max="5" width="6.84375" customWidth="1"/>
-    <col min="6" max="6" width="12.4609375" style="7" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="2"/>
+    <col min="2" max="2" width="16.625" customWidth="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
+    <col min="4" max="4" width="7.125" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2790,7 +2836,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>40442</v>
       </c>
@@ -2801,7 +2847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>40455</v>
       </c>
@@ -2833,33 +2879,33 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:Q17"/>
+  <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.61328125" customWidth="1"/>
-    <col min="2" max="2" width="24.4609375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="7.3828125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.625" customWidth="1"/>
+    <col min="2" max="2" width="24.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.84375" customWidth="1"/>
-    <col min="6" max="6" width="9.15234375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.4609375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.3828125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="6" max="6" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.4609375" style="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.15234375" style="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13" style="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="1.84375" style="15" customWidth="1"/>
-    <col min="15" max="15" width="10.15234375" style="15" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.4609375" style="15" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.15234375" style="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5" style="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.125" style="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13" style="22" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="1.875" style="15" customWidth="1"/>
+    <col min="15" max="15" width="10.125" style="15" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.5" style="15" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.125" style="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2906,7 +2952,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>112</v>
       </c>
@@ -2926,7 +2972,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>113</v>
       </c>
@@ -2946,7 +2992,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>114</v>
       </c>
@@ -2966,7 +3012,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>115</v>
       </c>
@@ -2986,7 +3032,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>116</v>
       </c>
@@ -3006,7 +3052,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>117</v>
       </c>
@@ -3017,7 +3063,7 @@
         <v>205</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="E7">
         <v>9</v>
@@ -3025,8 +3071,35 @@
       <c r="F7">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="G7">
+        <v>8</v>
+      </c>
+      <c r="H7">
+        <v>15</v>
+      </c>
+      <c r="I7" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="K7" s="21" t="s">
+        <v>210</v>
+      </c>
+      <c r="L7" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="M7" s="22" t="s">
+        <v>215</v>
+      </c>
+      <c r="O7" s="21" t="s">
+        <v>210</v>
+      </c>
+      <c r="P7" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q7" s="21" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>118</v>
       </c>
@@ -3046,7 +3119,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>121</v>
       </c>
@@ -3057,7 +3130,7 @@
         <v>205</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="E9">
         <v>16</v>
@@ -3065,23 +3138,60 @@
       <c r="F9">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="G9">
+        <v>12</v>
+      </c>
+      <c r="H9">
+        <v>20</v>
+      </c>
+      <c r="I9" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K9" s="21" t="s">
+        <v>210</v>
+      </c>
+      <c r="L9" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="M9" s="22" t="s">
+        <v>216</v>
+      </c>
+      <c r="O9" s="21" t="s">
+        <v>210</v>
+      </c>
+      <c r="P9" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q9" s="21" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B11" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B12" s="5"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B13" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B14" s="23" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" s="5" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="23" t="s">
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -3099,9 +3209,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3145,9 +3255,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3190,9 +3300,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3231,17 +3341,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.15234375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.4609375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>111</v>
       </c>
@@ -3252,7 +3362,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>112</v>
       </c>
@@ -3263,7 +3373,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>113</v>
       </c>
@@ -3274,7 +3384,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>114</v>
       </c>
@@ -3285,7 +3395,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>115</v>
       </c>
@@ -3296,7 +3406,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>116</v>
       </c>
@@ -3307,7 +3417,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>117</v>
       </c>
@@ -3318,7 +3428,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>118</v>
       </c>
@@ -3329,7 +3439,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>119</v>
       </c>
@@ -3340,7 +3450,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>120</v>
       </c>
@@ -3351,7 +3461,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>121</v>
       </c>
@@ -3362,7 +3472,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>122</v>
       </c>
@@ -3373,7 +3483,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>123</v>
       </c>
@@ -3384,7 +3494,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>124</v>
       </c>
@@ -3395,7 +3505,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>125</v>
       </c>
@@ -3406,7 +3516,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>126</v>
       </c>
@@ -3417,7 +3527,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
         <v>127</v>
       </c>
@@ -3428,7 +3538,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
         <v>128</v>
       </c>
@@ -3439,7 +3549,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>129</v>
       </c>
@@ -3450,7 +3560,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
         <v>130</v>
       </c>
@@ -3461,7 +3571,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
         <v>131</v>
       </c>
@@ -3472,7 +3582,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
         <v>132</v>
       </c>
@@ -3483,7 +3593,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>133</v>
       </c>
@@ -3494,7 +3604,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
         <v>134</v>
       </c>
@@ -3505,7 +3615,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
         <v>135</v>
       </c>
@@ -3516,7 +3626,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
         <v>136</v>
       </c>
@@ -3527,7 +3637,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" ht="126" x14ac:dyDescent="0.25">
       <c r="A27" s="19" t="s">
         <v>137</v>
       </c>
@@ -3538,7 +3648,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="19" t="s">
         <v>138</v>
       </c>
@@ -3549,7 +3659,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A29" s="19" t="s">
         <v>139</v>
       </c>
@@ -3560,7 +3670,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
         <v>140</v>
       </c>
@@ -3571,7 +3681,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
         <v>141</v>
       </c>
@@ -3582,7 +3692,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A32" s="19" t="s">
         <v>142</v>
       </c>
@@ -3593,7 +3703,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
         <v>143</v>
       </c>
@@ -3604,7 +3714,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
         <v>144</v>
       </c>
@@ -3615,7 +3725,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
         <v>145</v>
       </c>
@@ -3626,7 +3736,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A36" s="19" t="s">
         <v>146</v>
       </c>
@@ -3637,7 +3747,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A37" s="19" t="s">
         <v>147</v>
       </c>
@@ -3648,7 +3758,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A38" s="19" t="s">
         <v>148</v>
       </c>
@@ -3659,7 +3769,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A39" s="19" t="s">
         <v>149</v>
       </c>
@@ -3670,7 +3780,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A40" s="19" t="s">
         <v>150</v>
       </c>
@@ -3681,7 +3791,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A41" s="18" t="s">
         <v>151</v>
       </c>
@@ -3692,7 +3802,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A42" s="18" t="s">
         <v>152</v>
       </c>
@@ -3703,7 +3813,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A43" s="19" t="s">
         <v>153</v>
       </c>

</xml_diff>